<commit_message>
Revert "Merge pull request #41 from JokerQK/master"
This reverts commit f1381f00b6851fa4b04c6414c60432ef39bf671d, reversing
changes made to 25a832cece98ac09b336aaa6825caf5efbb89ddd.
</commit_message>
<xml_diff>
--- a/crawler_engine/result.xlsx
+++ b/crawler_engine/result.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>['2/20']</t>
+          <t>Week1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,7 +468,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>['2/20']</t>
+          <t>Week1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>